<commit_message>
small changes to urbs setup to create valid xlsx
</commit_message>
<xml_diff>
--- a/IDP_MapTool_Flask/pandapower2urbs/dataset/_transmission/test.xlsx
+++ b/IDP_MapTool_Flask/pandapower2urbs/dataset/_transmission/test.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="191">
   <si>
     <t>name</t>
   </si>
@@ -48,10 +48,10 @@
     <t>max_vm_pu</t>
   </si>
   <si>
-    <t>LVbus 1</t>
-  </si>
-  <si>
-    <t>MVbus 1</t>
+    <t>main_busbar</t>
+  </si>
+  <si>
+    <t>Trafostation_OS</t>
   </si>
   <si>
     <t>Connection Nodebus 138</t>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>controllable</t>
-  </si>
-  <si>
-    <t>load Household 0</t>
   </si>
   <si>
     <t>Load 137 household 1</t>
@@ -1140,72 +1137,72 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="B1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="R1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2">
         <v>110</v>
@@ -1256,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -1273,7 +1270,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3">
         <v>110</v>
@@ -1324,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S3">
         <v>0</v>
@@ -1354,13 +1351,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1374,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1388,7 +1385,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1402,7 +1399,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1416,7 +1413,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1430,7 +1427,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1444,7 +1441,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1458,7 +1455,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1466,13 +1463,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1480,13 +1477,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1494,13 +1491,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1508,13 +1505,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1522,13 +1519,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1536,13 +1533,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1550,13 +1547,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1564,13 +1561,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1578,13 +1575,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1592,13 +1589,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1606,13 +1603,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1620,13 +1617,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1634,13 +1631,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1648,13 +1645,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C22" t="s">
         <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1662,13 +1659,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1676,13 +1673,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1690,13 +1687,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1704,13 +1701,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1718,13 +1715,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1732,13 +1729,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1746,13 +1743,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1760,13 +1757,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1774,13 +1771,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1788,13 +1785,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1802,13 +1799,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1816,13 +1813,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C34" t="s">
         <v>21</v>
       </c>
       <c r="D34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1830,13 +1827,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C35" t="s">
         <v>22</v>
       </c>
       <c r="D35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1844,13 +1841,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
       </c>
       <c r="D36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1858,13 +1855,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C37" t="s">
         <v>24</v>
       </c>
       <c r="D37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1872,13 +1869,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1886,13 +1883,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1900,13 +1897,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C40" t="s">
         <v>25</v>
       </c>
       <c r="D40" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1914,13 +1911,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1928,13 +1925,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D42" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1942,13 +1939,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D43" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1956,13 +1953,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D44" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1970,13 +1967,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D45" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1984,13 +1981,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1998,13 +1995,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D47" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2012,13 +2009,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D48" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2026,13 +2023,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2040,13 +2037,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D50" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2054,13 +2051,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2068,13 +2065,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D52" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2082,13 +2079,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2096,13 +2093,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C54" t="s">
         <v>4</v>
       </c>
       <c r="D54" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2110,13 +2107,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C55" t="s">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2124,13 +2121,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2138,13 +2135,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D57" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2152,13 +2149,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D58" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2166,13 +2163,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C59" t="s">
         <v>19</v>
       </c>
       <c r="D59" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2180,13 +2177,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D60" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2194,13 +2191,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D61" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2208,13 +2205,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D62" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2222,13 +2219,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D63" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2236,13 +2233,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D64" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2250,13 +2247,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D65" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2264,13 +2261,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D66" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2278,13 +2275,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D67" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2292,13 +2289,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D68" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2306,13 +2303,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D69" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2320,13 +2317,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D70" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2334,13 +2331,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D71" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2348,13 +2345,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D72" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2362,13 +2359,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2376,13 +2373,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D74" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2390,13 +2387,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C75" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D75" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2404,13 +2401,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C76" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D76" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2418,13 +2415,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C77" t="s">
         <v>4</v>
       </c>
       <c r="D77" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2432,13 +2429,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C78" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D78" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2446,13 +2443,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D79" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2460,13 +2457,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C80" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D80" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2474,13 +2471,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C81" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D81" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2488,13 +2485,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
+        <v>178</v>
+      </c>
+      <c r="C82" t="s">
+        <v>82</v>
+      </c>
+      <c r="D82" t="s">
         <v>179</v>
-      </c>
-      <c r="C82" t="s">
-        <v>83</v>
-      </c>
-      <c r="D82" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2512,22 +2509,22 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>19</v>
@@ -2538,10 +2535,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" t="s">
         <v>190</v>
-      </c>
-      <c r="C2" t="s">
-        <v>191</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -2563,7 +2560,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2624,10 +2621,31 @@
         <v>26</v>
       </c>
       <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2">
+        <v>0.03</v>
       </c>
       <c r="P2" t="b">
         <v>1</v>
@@ -2641,7 +2659,7 @@
         <v>27</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -2662,50 +2680,12 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M3">
         <v>0.03</v>
       </c>
       <c r="P3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4">
-        <v>0.03</v>
-      </c>
-      <c r="P4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2730,28 +2710,28 @@
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>21</v>
@@ -2766,10 +2746,10 @@
         <v>24</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>25</v>
@@ -2780,7 +2760,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2819,37 +2799,37 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>2</v>
@@ -2863,10 +2843,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -2907,10 +2887,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -2951,10 +2931,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -2995,10 +2975,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
         <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>55</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3052,73 +3032,73 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -3126,10 +3106,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
         <v>74</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3162,7 +3142,7 @@
         <v>150</v>
       </c>
       <c r="N2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -3210,16 +3190,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3305,13 +3285,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3398,30 +3378,30 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2">
         <v>0.642</v>
@@ -3439,7 +3419,7 @@
         <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I2">
         <v>0.00403</v>
@@ -3447,7 +3427,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3">
         <v>0.225</v>
@@ -3465,7 +3445,7 @@
         <v>120</v>
       </c>
       <c r="H3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I3">
         <v>0.00403</v>
@@ -3473,7 +3453,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4">
         <v>0.208</v>
@@ -3491,7 +3471,7 @@
         <v>150</v>
       </c>
       <c r="H4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I4">
         <v>0.00403</v>
@@ -3499,7 +3479,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5">
         <v>0.313</v>
@@ -3517,7 +3497,7 @@
         <v>95</v>
       </c>
       <c r="H5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I5">
         <v>0.00403</v>
@@ -3525,7 +3505,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6">
         <v>0.161</v>
@@ -3543,7 +3523,7 @@
         <v>185</v>
       </c>
       <c r="H6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I6">
         <v>0.00403</v>
@@ -3551,7 +3531,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7">
         <v>0.122</v>
@@ -3569,7 +3549,7 @@
         <v>240</v>
       </c>
       <c r="H7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I7">
         <v>0.00403</v>
@@ -3577,7 +3557,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8">
         <v>0.313</v>
@@ -3595,7 +3575,7 @@
         <v>95</v>
       </c>
       <c r="H8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I8">
         <v>0.00403</v>
@@ -3603,7 +3583,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9">
         <v>0.161</v>
@@ -3621,7 +3601,7 @@
         <v>185</v>
       </c>
       <c r="H9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I9">
         <v>0.00403</v>
@@ -3629,7 +3609,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10">
         <v>0.122</v>
@@ -3647,7 +3627,7 @@
         <v>240</v>
       </c>
       <c r="H10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I10">
         <v>0.00403</v>
@@ -3655,7 +3635,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11">
         <v>0.206</v>
@@ -3673,7 +3653,7 @@
         <v>150</v>
       </c>
       <c r="H11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I11">
         <v>0.00403</v>
@@ -3681,7 +3661,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12">
         <v>0.253</v>
@@ -3699,7 +3679,7 @@
         <v>120</v>
       </c>
       <c r="H12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I12">
         <v>0.00403</v>
@@ -3707,7 +3687,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13">
         <v>0.443</v>
@@ -3725,7 +3705,7 @@
         <v>70</v>
       </c>
       <c r="H13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I13">
         <v>0.00403</v>
@@ -3733,7 +3713,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14">
         <v>0.206</v>
@@ -3751,7 +3731,7 @@
         <v>150</v>
       </c>
       <c r="H14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I14">
         <v>0.00403</v>
@@ -3759,7 +3739,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C15">
         <v>0.253</v>
@@ -3777,7 +3757,7 @@
         <v>120</v>
       </c>
       <c r="H15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I15">
         <v>0.00403</v>
@@ -3785,7 +3765,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16">
         <v>0.443</v>
@@ -3803,7 +3783,7 @@
         <v>70</v>
       </c>
       <c r="H16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I16">
         <v>0.00403</v>
@@ -3811,7 +3791,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17">
         <v>0.153</v>
@@ -3829,7 +3809,7 @@
         <v>120</v>
       </c>
       <c r="H17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I17">
         <v>0.00393</v>
@@ -3837,7 +3817,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18">
         <v>0.099</v>
@@ -3855,7 +3835,7 @@
         <v>185</v>
       </c>
       <c r="H18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I18">
         <v>0.00393</v>
@@ -3863,7 +3843,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19">
         <v>0.075</v>
@@ -3881,7 +3861,7 @@
         <v>240</v>
       </c>
       <c r="H19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I19">
         <v>0.00393</v>
@@ -3889,7 +3869,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20">
         <v>0.06</v>
@@ -3907,7 +3887,7 @@
         <v>300</v>
       </c>
       <c r="H20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I20">
         <v>0.00393</v>
@@ -3915,7 +3895,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C21">
         <v>1.8769</v>
@@ -3933,7 +3913,7 @@
         <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I21">
         <v>0.00403</v>
@@ -3941,7 +3921,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22">
         <v>1.2012</v>
@@ -3959,7 +3939,7 @@
         <v>24</v>
       </c>
       <c r="H22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I22">
         <v>0.00403</v>
@@ -3967,7 +3947,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C23">
         <v>0.5939</v>
@@ -3985,7 +3965,7 @@
         <v>48</v>
       </c>
       <c r="H23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I23">
         <v>0.00403</v>
@@ -3993,7 +3973,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C24">
         <v>0.306</v>
@@ -4011,7 +3991,7 @@
         <v>94</v>
       </c>
       <c r="H24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I24">
         <v>0.00403</v>
@@ -4019,7 +3999,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25">
         <v>0.8342000000000001</v>
@@ -4037,7 +4017,7 @@
         <v>34</v>
       </c>
       <c r="H25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I25">
         <v>0.00403</v>
@@ -4045,7 +4025,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26">
         <v>0.5939</v>
@@ -4063,7 +4043,7 @@
         <v>48</v>
       </c>
       <c r="H26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I26">
         <v>0.00403</v>
@@ -4071,7 +4051,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C27">
         <v>0.4132</v>
@@ -4089,7 +4069,7 @@
         <v>70</v>
       </c>
       <c r="H27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I27">
         <v>0.00403</v>
@@ -4097,7 +4077,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C28">
         <v>0.306</v>
@@ -4115,7 +4095,7 @@
         <v>94</v>
       </c>
       <c r="H28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I28">
         <v>0.00403</v>
@@ -4123,7 +4103,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C29">
         <v>0.2376</v>
@@ -4141,7 +4121,7 @@
         <v>122</v>
       </c>
       <c r="H29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I29">
         <v>0.00403</v>
@@ -4149,7 +4129,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C30">
         <v>0.194</v>
@@ -4167,7 +4147,7 @@
         <v>149</v>
       </c>
       <c r="H30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I30">
         <v>0.00403</v>
@@ -4175,7 +4155,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C31">
         <v>0.8342000000000001</v>
@@ -4193,7 +4173,7 @@
         <v>34</v>
       </c>
       <c r="H31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I31">
         <v>0.00403</v>
@@ -4201,7 +4181,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C32">
         <v>0.5939</v>
@@ -4219,7 +4199,7 @@
         <v>48</v>
       </c>
       <c r="H32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I32">
         <v>0.00403</v>
@@ -4227,7 +4207,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C33">
         <v>0.4132</v>
@@ -4245,7 +4225,7 @@
         <v>70</v>
       </c>
       <c r="H33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I33">
         <v>0.00403</v>
@@ -4253,7 +4233,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C34">
         <v>0.306</v>
@@ -4271,7 +4251,7 @@
         <v>94</v>
       </c>
       <c r="H34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I34">
         <v>0.00403</v>
@@ -4279,7 +4259,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35">
         <v>0.2376</v>
@@ -4297,7 +4277,7 @@
         <v>122</v>
       </c>
       <c r="H35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I35">
         <v>0.00403</v>
@@ -4305,7 +4285,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C36">
         <v>0.194</v>
@@ -4323,7 +4303,7 @@
         <v>149</v>
       </c>
       <c r="H36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I36">
         <v>0.00403</v>
@@ -4331,7 +4311,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C37">
         <v>0.1571</v>
@@ -4349,7 +4329,7 @@
         <v>184</v>
       </c>
       <c r="H37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I37">
         <v>0.00403</v>
@@ -4357,7 +4337,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C38">
         <v>0.1188</v>
@@ -4375,7 +4355,7 @@
         <v>243</v>
       </c>
       <c r="H38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I38">
         <v>0.00403</v>
@@ -4383,7 +4363,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C39">
         <v>0.5939</v>
@@ -4401,7 +4381,7 @@
         <v>48</v>
       </c>
       <c r="H39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I39">
         <v>0.00403</v>
@@ -4409,7 +4389,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C40">
         <v>0.4132</v>
@@ -4427,7 +4407,7 @@
         <v>70</v>
       </c>
       <c r="H40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I40">
         <v>0.00403</v>
@@ -4435,7 +4415,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C41">
         <v>0.306</v>
@@ -4453,7 +4433,7 @@
         <v>94</v>
       </c>
       <c r="H41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I41">
         <v>0.00403</v>
@@ -4461,7 +4441,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C42">
         <v>0.2376</v>
@@ -4479,7 +4459,7 @@
         <v>122</v>
       </c>
       <c r="H42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I42">
         <v>0.00403</v>
@@ -4487,7 +4467,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C43">
         <v>0.194</v>
@@ -4505,7 +4485,7 @@
         <v>149</v>
       </c>
       <c r="H43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I43">
         <v>0.00403</v>
@@ -4513,7 +4493,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C44">
         <v>0.1571</v>
@@ -4531,7 +4511,7 @@
         <v>184</v>
       </c>
       <c r="H44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I44">
         <v>0.00403</v>
@@ -4539,7 +4519,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C45">
         <v>0.1188</v>
@@ -4557,7 +4537,7 @@
         <v>243</v>
       </c>
       <c r="H45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I45">
         <v>0.00403</v>
@@ -4565,7 +4545,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C46">
         <v>0.0949</v>
@@ -4583,7 +4563,7 @@
         <v>305</v>
       </c>
       <c r="H46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I46">
         <v>0.00403</v>
@@ -4591,7 +4571,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C47">
         <v>0.059</v>
@@ -4609,7 +4589,7 @@
         <v>490</v>
       </c>
       <c r="H47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I47">
         <v>0.00403</v>
@@ -4617,7 +4597,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C48">
         <v>0.042</v>
@@ -4635,7 +4615,7 @@
         <v>679</v>
       </c>
       <c r="H48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I48">
         <v>0.00403</v>
@@ -4643,7 +4623,7 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C49">
         <v>0.059</v>
@@ -4661,7 +4641,7 @@
         <v>490</v>
       </c>
       <c r="H49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I49">
         <v>0.00403</v>
@@ -4669,7 +4649,7 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C50">
         <v>0.042</v>
@@ -4687,7 +4667,7 @@
         <v>679</v>
       </c>
       <c r="H50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I50">
         <v>0.00403</v>
@@ -4695,7 +4675,7 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C51">
         <v>0.059</v>
@@ -4713,7 +4693,7 @@
         <v>490</v>
       </c>
       <c r="H51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I51">
         <v>0.00403</v>
@@ -4721,7 +4701,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C52">
         <v>0.042</v>
@@ -4739,7 +4719,7 @@
         <v>679</v>
       </c>
       <c r="H52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I52">
         <v>0.00403</v>
@@ -4747,7 +4727,7 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C53">
         <v>1.15</v>
@@ -4767,7 +4747,7 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C54">
         <v>0.524</v>
@@ -4787,7 +4767,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C55">
         <v>0.164</v>
@@ -4807,7 +4787,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C56">
         <v>0.32</v>
@@ -4827,7 +4807,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C57">
         <v>0.268</v>
@@ -4847,7 +4827,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C58">
         <v>0.193</v>
@@ -4886,51 +4866,51 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2">
         <v>160</v>
@@ -4957,7 +4937,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -4980,7 +4960,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -5007,7 +4987,7 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -5030,7 +5010,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C4">
         <v>63</v>
@@ -5057,7 +5037,7 @@
         <v>150</v>
       </c>
       <c r="K4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -5080,7 +5060,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5">
         <v>40</v>
@@ -5107,7 +5087,7 @@
         <v>150</v>
       </c>
       <c r="K5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -5130,7 +5110,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C6">
         <v>25</v>
@@ -5157,7 +5137,7 @@
         <v>150</v>
       </c>
       <c r="K6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -5180,7 +5160,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C7">
         <v>63</v>
@@ -5207,7 +5187,7 @@
         <v>150</v>
       </c>
       <c r="K7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -5230,7 +5210,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C8">
         <v>40</v>
@@ -5257,7 +5237,7 @@
         <v>150</v>
       </c>
       <c r="K8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -5280,7 +5260,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9">
         <v>25</v>
@@ -5307,7 +5287,7 @@
         <v>150</v>
       </c>
       <c r="K9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -5330,7 +5310,7 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10">
         <v>0.25</v>
@@ -5357,7 +5337,7 @@
         <v>150</v>
       </c>
       <c r="K10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -5380,7 +5360,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11">
         <v>0.4</v>
@@ -5407,7 +5387,7 @@
         <v>150</v>
       </c>
       <c r="K11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -5430,7 +5410,7 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C12">
         <v>0.63</v>
@@ -5457,7 +5437,7 @@
         <v>150</v>
       </c>
       <c r="K12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -5480,7 +5460,7 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C13">
         <v>0.25</v>
@@ -5507,7 +5487,7 @@
         <v>150</v>
       </c>
       <c r="K13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -5530,7 +5510,7 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14">
         <v>0.4</v>
@@ -5557,7 +5537,7 @@
         <v>150</v>
       </c>
       <c r="K14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -5580,7 +5560,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C15">
         <v>0.63</v>
@@ -5607,7 +5587,7 @@
         <v>150</v>
       </c>
       <c r="K15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L15">
         <v>0</v>

</xml_diff>